<commit_message>
v1 three pages. not good
</commit_message>
<xml_diff>
--- a/static/Text for scorecard.xlsx
+++ b/static/Text for scorecard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/mdesimone_worldbank_org/Documents/Scorecard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb384996\OneDrive - WBG\WorldBank\CHI_AM19_scorecard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="106" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{343D0034-B9A7-412C-9B69-2A48FDA3F5E1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content" sheetId="1" r:id="rId1"/>
@@ -6545,13 +6545,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6869,8 +6869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB593C5-CB33-4C82-8892-16AD6BBB74CF}">
   <dimension ref="A1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7682,8 +7682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF53BE-D705-4843-87FF-A6CBC631D5C8}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7693,13 +7693,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -7719,13 +7719,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7796,13 +7796,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -7873,13 +7873,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -8070,13 +8070,13 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -8186,13 +8186,13 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -8212,13 +8212,13 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -8289,13 +8289,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -8366,13 +8366,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -8562,13 +8562,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
@@ -8711,16 +8711,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A60:E60"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A60:E60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8734,15 +8734,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF3981026596CA4B849E701D3DDF780C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c49eee62a26e7687f17b4c71c2f154f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b9a0195-bf3a-44f4-98cb-18d4a789a435" xmlns:ns4="52fb1372-aa68-4a6d-be04-392fdfd269a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b001afaec740ebb1a4e695ae3c47413d" ns3:_="" ns4:_="">
     <xsd:import namespace="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
@@ -8957,32 +8948,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2655F4-972B-4D4C-81F2-9F7116C52A0F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
+    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6311E5-01A1-4FC1-932F-966E25ED6D02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8999,4 +8991,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add row filters to xlsx file... not important
</commit_message>
<xml_diff>
--- a/static/Text for scorecard.xlsx
+++ b/static/Text for scorecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb384996\OneDrive - WBG\WorldBank\CHI_AM19_scorecard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{343D0034-B9A7-412C-9B69-2A48FDA3F5E1}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{846D1036-453A-4176-A322-7EBC3D043F69}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
   </bookViews>
@@ -6545,13 +6545,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7682,24 +7682,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF53BE-D705-4843-87FF-A6CBC631D5C8}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="41" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -7719,13 +7719,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7761,7 +7761,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>169</v>
       </c>
@@ -7795,16 +7795,16 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>154</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>159</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>164</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>169</v>
       </c>
@@ -7872,16 +7872,16 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>192</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>197</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>202</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>207</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>212</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>217</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>222</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>227</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>232</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>237</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>242</v>
       </c>
@@ -8069,16 +8069,16 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>248</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>253</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>258</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>263</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>268</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>273</v>
       </c>
@@ -8180,19 +8180,20 @@
         <v>277</v>
       </c>
     </row>
+    <row r="32" spans="1:6" collapsed="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -8212,13 +8213,13 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -8289,13 +8290,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -8366,13 +8367,13 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -8562,13 +8563,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
@@ -8711,16 +8712,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8734,6 +8735,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF3981026596CA4B849E701D3DDF780C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c49eee62a26e7687f17b4c71c2f154f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b9a0195-bf3a-44f4-98cb-18d4a789a435" xmlns:ns4="52fb1372-aa68-4a6d-be04-392fdfd269a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b001afaec740ebb1a4e695ae3c47413d" ns3:_="" ns4:_="">
     <xsd:import namespace="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
@@ -8948,33 +8958,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2655F4-972B-4D4C-81F2-9F7116C52A0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
-    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6311E5-01A1-4FC1-932F-966E25ED6D02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8991,12 +9000,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update file for easiness to read
</commit_message>
<xml_diff>
--- a/static/Text for scorecard.xlsx
+++ b/static/Text for scorecard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb384996\OneDrive - WBG\WorldBank\CHI_AM19_scorecard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{846D1036-453A-4176-A322-7EBC3D043F69}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{B1C8B596-B897-426D-913C-087E67FA38B6}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
   </bookViews>
@@ -3796,9 +3796,6 @@
     <t>Difference with DO for region</t>
   </si>
   <si>
-    <t xml:space="preserve">do_performance_hd_diffmr </t>
-  </si>
-  <si>
     <t xml:space="preserve">do_performance_edu_diffmr </t>
   </si>
   <si>
@@ -6440,6 +6437,9 @@
   </si>
   <si>
     <t>if lastafr==.</t>
+  </si>
+  <si>
+    <t>do_performance_hd_diffmr</t>
   </si>
 </sst>
 </file>
@@ -6545,13 +6545,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6969,7 +6969,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7012,7 +7012,7 @@
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7055,10 +7055,10 @@
     </row>
     <row r="19" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="20" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7098,10 +7098,10 @@
     </row>
     <row r="24" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7141,10 +7141,10 @@
     </row>
     <row r="29" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7184,10 +7184,10 @@
     </row>
     <row r="34" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7227,10 +7227,10 @@
     </row>
     <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7263,7 +7263,7 @@
         <v>85</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7271,7 +7271,7 @@
         <v>86</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7292,10 +7292,10 @@
     </row>
     <row r="46" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7306,7 +7306,7 @@
         <v>92</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7314,7 +7314,7 @@
         <v>93</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7335,10 +7335,10 @@
     </row>
     <row r="51" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7349,7 +7349,7 @@
         <v>99</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7357,7 +7357,7 @@
         <v>100</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7378,10 +7378,10 @@
     </row>
     <row r="56" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7392,7 +7392,7 @@
         <v>106</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7400,15 +7400,15 @@
         <v>107</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7419,7 +7419,7 @@
         <v>109</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7427,7 +7427,7 @@
         <v>110</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7451,7 +7451,7 @@
         <v>115</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7459,7 +7459,7 @@
         <v>116</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7475,15 +7475,15 @@
         <v>119</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7494,7 +7494,7 @@
         <v>121</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7502,7 +7502,7 @@
         <v>122</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7510,7 +7510,7 @@
         <v>123</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7518,15 +7518,15 @@
         <v>124</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7537,7 +7537,7 @@
         <v>126</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7545,7 +7545,7 @@
         <v>127</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7553,7 +7553,7 @@
         <v>128</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7561,15 +7561,15 @@
         <v>129</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D78" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7580,7 +7580,7 @@
         <v>5</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7682,8 +7682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF53BE-D705-4843-87FF-A6CBC631D5C8}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -7693,13 +7693,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -7719,13 +7719,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -7761,7 +7761,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>169</v>
       </c>
@@ -7795,16 +7795,16 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>154</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>159</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>164</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>169</v>
       </c>
@@ -7872,16 +7872,16 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>192</v>
       </c>
@@ -7898,302 +7898,301 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>197</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="E15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="E16" s="7" t="s">
+    </row>
+    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E18" s="7" t="s">
+    </row>
+    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="E19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="E20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="E21" s="8" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="E22" s="7" t="s">
+    </row>
+    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E23" s="7" t="s">
+    </row>
+    <row r="24" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E24" s="7" t="s">
+    </row>
+    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B26" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="E26" s="7" t="s">
+    </row>
+    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B27" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E27" s="8" t="s">
+    </row>
+    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="E28" s="8" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E29" s="7" t="s">
+    </row>
+    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="E30" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="E30" s="7" t="s">
+    </row>
+    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" collapsed="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
@@ -8213,29 +8212,29 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>154</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -8243,16 +8242,16 @@
         <v>159</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="D40" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="E40" s="12" t="s">
         <v>282</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -8260,16 +8259,16 @@
         <v>164</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -8277,42 +8276,42 @@
         <v>169</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>154</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -8320,16 +8319,16 @@
         <v>159</v>
       </c>
       <c r="B45" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="E45" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -8337,16 +8336,16 @@
         <v>164</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -8354,42 +8353,42 @@
         <v>169</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>192</v>
       </c>
       <c r="B49" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="D49" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="E49" s="12" t="s">
         <v>290</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -8397,331 +8396,328 @@
         <v>197</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B53" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="D53" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="E53" s="12" t="s">
         <v>294</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B57" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="D57" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
+      <c r="A60" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B61" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="C61" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="D61" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="E61" s="12" t="s">
         <v>298</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B64" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C64" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="D64" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="E64" s="12" t="s">
         <v>302</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>312</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="7">
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8735,15 +8731,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF3981026596CA4B849E701D3DDF780C" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c49eee62a26e7687f17b4c71c2f154f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2b9a0195-bf3a-44f4-98cb-18d4a789a435" xmlns:ns4="52fb1372-aa68-4a6d-be04-392fdfd269a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b001afaec740ebb1a4e695ae3c47413d" ns3:_="" ns4:_="">
     <xsd:import namespace="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
@@ -8958,32 +8945,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2655F4-972B-4D4C-81F2-9F7116C52A0F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E6311E5-01A1-4FC1-932F-966E25ED6D02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9000,4 +8988,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
graphs without edu data produced
</commit_message>
<xml_diff>
--- a/static/Text for scorecard.xlsx
+++ b/static/Text for scorecard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb384996\OneDrive - WBG\WorldBank\CHI_AM19_scorecard\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB538904\OneDrive - WBG\CHI_AM19_scorecard\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{B1C8B596-B897-426D-913C-087E67FA38B6}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{00623372-AF1B-47B5-9E0A-0E09EA7A00D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{BECF4AC3-0914-4A91-B374-AB35F0C0CC82}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230" activeTab="1" xr2:uid="{32D3B10D-A585-47FA-99EC-0BDDC3749A17}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Content" sheetId="1" r:id="rId1"/>
@@ -6545,13 +6545,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6873,16 +6873,16 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="125.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="31.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="125.54296875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
@@ -6940,7 +6940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>37</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="2" t="s">
         <v>39</v>
       </c>
@@ -7045,7 +7045,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
@@ -7053,7 +7053,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>314</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="20" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>43</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
@@ -7088,7 +7088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="2" t="s">
         <v>50</v>
       </c>
@@ -7096,7 +7096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="2" t="s">
         <v>359</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>52</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="2" t="s">
         <v>55</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" s="2" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="2" t="s">
         <v>57</v>
       </c>
@@ -7131,7 +7131,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="2" t="s">
         <v>59</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="2" t="s">
         <v>317</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="2" t="s">
         <v>64</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>66</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>68</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C34" s="2" t="s">
         <v>319</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>70</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C37" s="2" t="s">
         <v>75</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C38" s="2" t="s">
         <v>77</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
         <v>321</v>
       </c>
@@ -7233,7 +7233,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C41" s="2" t="s">
         <v>82</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
         <v>84</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C43" s="2" t="s">
         <v>86</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C44" s="2" t="s">
         <v>87</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C45" s="2" t="s">
         <v>89</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="2" t="s">
         <v>323</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="2" t="s">
         <v>93</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="2" t="s">
         <v>94</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C50" s="2" t="s">
         <v>96</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="2" t="s">
         <v>328</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>98</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C53" s="2" t="s">
         <v>100</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C54" s="2" t="s">
         <v>101</v>
       </c>
@@ -7368,7 +7368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C55" s="2" t="s">
         <v>103</v>
       </c>
@@ -7376,7 +7376,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C56" s="2" t="s">
         <v>331</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="57" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>105</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="58" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C58" s="2" t="s">
         <v>107</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C59" s="2" t="s">
         <v>333</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="1" t="s">
         <v>108</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C61" s="2" t="s">
         <v>110</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C62" s="2" t="s">
         <v>111</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C63" s="2" t="s">
         <v>113</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C64" s="2" t="s">
         <v>115</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C65" s="2" t="s">
         <v>116</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C66" s="2" t="s">
         <v>117</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C67" s="2" t="s">
         <v>119</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C68" s="2" t="s">
         <v>344</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="1" t="s">
         <v>120</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C70" s="2" t="s">
         <v>122</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C71" s="2" t="s">
         <v>123</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C72" s="2" t="s">
         <v>124</v>
       </c>
@@ -7521,7 +7521,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C73" s="2" t="s">
         <v>347</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
         <v>125</v>
       </c>
@@ -7540,7 +7540,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C75" s="2" t="s">
         <v>127</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C76" s="2" t="s">
         <v>128</v>
       </c>
@@ -7556,7 +7556,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C77" s="2" t="s">
         <v>129</v>
       </c>
@@ -7564,7 +7564,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C78" s="2" t="s">
         <v>357</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="1" t="s">
         <v>130</v>
       </c>
@@ -7583,7 +7583,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>131</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>133</v>
       </c>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="D81" s="13"/>
     </row>
-    <row r="82" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>135</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
       <c r="C83" s="4" t="s">
         <v>138</v>
@@ -7626,7 +7626,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="3" t="s">
         <v>140</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="3"/>
       <c r="C85" s="3" t="s">
         <v>143</v>
@@ -7646,7 +7646,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>145</v>
       </c>
@@ -7657,18 +7657,18 @@
         <v>146</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="33.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C81:D81"/>
@@ -7682,26 +7682,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FF53BE-D705-4843-87FF-A6CBC631D5C8}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="5" width="41" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>148</v>
       </c>
@@ -7718,16 +7718,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>154</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>159</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>169</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>174</v>
       </c>
@@ -7804,7 +7804,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>154</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>159</v>
       </c>
@@ -7838,7 +7838,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>164</v>
       </c>
@@ -7855,7 +7855,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>169</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>191</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>192</v>
       </c>
@@ -7898,7 +7898,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>197</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>201</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>206</v>
       </c>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>211</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>216</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>221</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>226</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>231</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>236</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>241</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>246</v>
       </c>
@@ -8078,7 +8078,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>247</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>252</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>257</v>
       </c>
@@ -8129,7 +8129,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>262</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>267</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>272</v>
       </c>
@@ -8180,21 +8180,21 @@
         <v>276</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>148</v>
       </c>
@@ -8211,16 +8211,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>154</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>159</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>164</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>169</v>
       </c>
@@ -8288,16 +8288,16 @@
         <v>278</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>154</v>
       </c>
@@ -8314,7 +8314,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>159</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>164</v>
       </c>
@@ -8348,7 +8348,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>169</v>
       </c>
@@ -8365,16 +8365,16 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+    </row>
+    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>192</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>197</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>206</v>
       </c>
@@ -8442,7 +8442,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>211</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>216</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>226</v>
       </c>
@@ -8510,7 +8510,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>231</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="11" t="s">
         <v>236</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>241</v>
       </c>
@@ -8561,16 +8561,16 @@
         <v>278</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-    </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+    </row>
+    <row r="61" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>247</v>
       </c>
@@ -8587,7 +8587,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>252</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>257</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>262</v>
       </c>
@@ -8638,7 +8638,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>267</v>
       </c>
@@ -8655,7 +8655,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>272</v>
       </c>
@@ -8672,12 +8672,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>304</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>306</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>308</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>310</v>
       </c>
@@ -8711,13 +8711,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -8725,9 +8725,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8946,27 +8949,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2655F4-972B-4D4C-81F2-9F7116C52A0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8991,9 +8982,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8036B806-D167-4DA8-8E58-94F593C603F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C2655F4-972B-4D4C-81F2-9F7116C52A0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="2b9a0195-bf3a-44f4-98cb-18d4a789a435"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="52fb1372-aa68-4a6d-be04-392fdfd269a8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>